<commit_message>
Sleep analysis doing correlation. Also got some before/after van stats.
</commit_message>
<xml_diff>
--- a/database_schema.xlsx
+++ b/database_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackiekinsler/projects/sleep_analysis_py/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E674BE7-5A67-824B-88D5-4FA02F0BC8D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CDC220-55F5-2744-899A-EC3181E63E84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39180" yWindow="2640" windowWidth="27640" windowHeight="16540" xr2:uid="{CD9CC61B-9E7C-2442-9A39-070D7DADF086}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
   <si>
     <t>HEARTRATE</t>
   </si>
@@ -42,9 +42,6 @@
     <t>every 5 seconds</t>
   </si>
   <si>
-    <t>SLEEEP_DETAIL</t>
-  </si>
-  <si>
     <t>startTime</t>
   </si>
   <si>
@@ -205,6 +202,51 @@
   </si>
   <si>
     <t xml:space="preserve">new table on right </t>
+  </si>
+  <si>
+    <t>summary.deep.count</t>
+  </si>
+  <si>
+    <t>summary.deep.minutes</t>
+  </si>
+  <si>
+    <t>summary.deep.thirtyDayAvgMinutes</t>
+  </si>
+  <si>
+    <t>summary.wake.count</t>
+  </si>
+  <si>
+    <t>summary.wake.minutes</t>
+  </si>
+  <si>
+    <t>summary.wake.thirtyDayAvgMinutes</t>
+  </si>
+  <si>
+    <t>summary.light.count</t>
+  </si>
+  <si>
+    <t>summary.light.minutes</t>
+  </si>
+  <si>
+    <t>summary.light.thirtyDayAvgMinutes</t>
+  </si>
+  <si>
+    <t>summary.rem.count</t>
+  </si>
+  <si>
+    <t>summary.rem.minutes</t>
+  </si>
+  <si>
+    <t>summary.rem.thirtyDayAvgMinutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lots of nested data here </t>
+  </si>
+  <si>
+    <t>SLEEP_NESTED</t>
+  </si>
+  <si>
+    <t>SLEEP_DETAIL</t>
   </si>
 </sst>
 </file>
@@ -368,13 +410,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -412,6 +455,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E31136-5511-DC46-8E73-8340A4518620}">
-  <dimension ref="B2:Q49"/>
+  <dimension ref="B2:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F13" sqref="F13:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,19 +782,19 @@
     <col min="2" max="3" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:21" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="G2" s="26"/>
+      <c r="G2" s="27"/>
       <c r="H2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M2" s="19"/>
-    </row>
-    <row r="3" spans="2:17" ht="17" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="M2" s="20"/>
+    </row>
+    <row r="3" spans="2:21" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -760,101 +805,101 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" s="19"/>
-    </row>
-    <row r="4" spans="2:17" ht="17" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="M3" s="20"/>
+    </row>
+    <row r="4" spans="2:21" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="M4" s="19"/>
-    </row>
-    <row r="5" spans="2:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="M4" s="20"/>
+    </row>
+    <row r="5" spans="2:21" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="20"/>
+    </row>
+    <row r="6" spans="2:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="19"/>
-    </row>
-    <row r="6" spans="2:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="M6" s="19"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="s">
+      <c r="M6" s="20"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="10"/>
+    </row>
+    <row r="10" spans="2:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9"/>
-    </row>
-    <row r="10" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="E10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="M10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="N10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="O10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="P10" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="Q10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -869,324 +914,415 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
+      <c r="P11" s="29" t="s">
+        <v>71</v>
+      </c>
       <c r="Q11" s="1"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B14" s="13" t="s">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="F13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="10"/>
+    </row>
+    <row r="14" spans="2:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B19" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="2:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="L25" s="20"/>
+    </row>
+    <row r="26" spans="2:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="L26" s="20"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B27" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="24"/>
+      <c r="L27" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="10"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B28" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+      <c r="C28" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="J28" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B32" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="E32" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="19"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="19"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="2:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="L20" s="19"/>
-    </row>
-    <row r="21" spans="2:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="L21" s="19"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B22" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="23"/>
-      <c r="L22" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="9"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B23" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="J23" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N23" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="O23" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B27" s="6" t="s">
+      <c r="C37" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="E27" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" s="18"/>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B31" s="6" t="s">
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="13"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="18"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B32" s="15" t="s">
+      <c r="C40" s="19"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+      <c r="C41" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="13"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="19"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="12"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="18"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="15" t="s">
+      <c r="C46" s="13"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="19"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="10" t="s">
+      <c r="C49" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="12"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="6" t="s">
+      <c r="C50" s="13"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="18"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" s="12"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="6" t="s">
+      <c r="C52" s="8"/>
+      <c r="D52" s="19"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="18"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" s="12"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="18"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="12"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B54" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" s="12"/>
+      <c r="D54" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B22:D22"/>
+  <mergeCells count="13">
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B27:D27"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="F13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>